<commit_message>
optimised coin counting interval
extended intervall (from 135ms to 140 ms) to support newer coin counter hardware. New effort estimations.
</commit_message>
<xml_diff>
--- a/Aufwandschätzung.xlsx
+++ b/Aufwandschätzung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gesichert\GitHub\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80404F92-0F5E-4210-95CE-9FF8DB02CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06A4924-12C6-4DF3-8352-B020F868B39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F0280D5-7879-4722-A320-08298A157B18}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Fächer</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Bohren, Dübeln, Leimen Boden &amp; Seitenteile</t>
   </si>
   <si>
-    <t>Bohren, Dübeln, Leimen / Einpassen Rückkwand inkl. Kabeldurchführung</t>
-  </si>
-  <si>
     <t>Einsetzen Klavierband, Montage Klappe, Einsetzen Verriegelung, Ausschneiden Führung der Verriegelung</t>
   </si>
   <si>
@@ -167,13 +164,21 @@
     <t>Aufwand Honigautomat (5 Fächer, Solar)</t>
   </si>
   <si>
-    <t>Stunden</t>
-  </si>
-  <si>
     <t>Bereich</t>
   </si>
   <si>
     <t>Planung, Koordination, Abstimmung, Kommunikation, Teilebeschaffung, Dokumentation</t>
+  </si>
+  <si>
+    <t>Bohren, Dübeln, Leimen / Einpassen Rückwand inkl. Kabeldurchführung</t>
+  </si>
+  <si>
+    <t>Stunden
+min</t>
+  </si>
+  <si>
+    <t>Stunden
+max</t>
   </si>
 </sst>
 </file>
@@ -217,12 +222,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -265,7 +273,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C9B2A3AC-D634-4792-8F44-EC23E16BFB2D}" name="Bereich"/>
     <tableColumn id="2" xr3:uid="{4A066264-8590-452F-8AEF-62180E0C1C14}" name="Aufwand Honigautomat (5 Fächer, Solar)"/>
-    <tableColumn id="3" xr3:uid="{D54DC5BE-55E5-4600-A02B-A907B412CF14}" name="Stunden"/>
+    <tableColumn id="3" xr3:uid="{D54DC5BE-55E5-4600-A02B-A907B412CF14}" name="Stunden_x000a_min"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -568,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B5A164-1C07-45DA-B043-47109C77269A}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,18 +588,21 @@
     <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -599,10 +610,13 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -610,10 +624,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -621,10 +638,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -632,32 +652,41 @@
         <v>4</v>
       </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -665,10 +694,13 @@
         <v>6</v>
       </c>
       <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -678,8 +710,11 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -687,21 +722,27 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -709,10 +750,13 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -722,8 +766,11 @@
       <c r="C13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -731,10 +778,13 @@
         <v>14</v>
       </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -742,32 +792,41 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -775,10 +834,13 @@
         <v>18</v>
       </c>
       <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -786,10 +848,13 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -797,10 +862,13 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -808,21 +876,27 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -830,105 +904,141 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
       <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
         <f>SUM(C1:C32)</f>
+        <v>21.5</v>
+      </c>
+      <c r="D33" s="2">
+        <f>SUM(D1:D32)</f>
         <v>36</v>
+      </c>
+      <c r="E33">
+        <f>(D33+Tabelle2[[#This Row],[Stunden
+min]])/2</f>
+        <v>28.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>